<commit_message>
hoja con diferencias entre partidos (max y min) y hoja con tabla de partidos acumulados
</commit_message>
<xml_diff>
--- a/frances.xlsx
+++ b/frances.xlsx
@@ -8,14 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Fixture frances" sheetId="1" r:id="rId1"/>
-    <sheet name="Breaks" sheetId="2" r:id="rId2"/>
+    <sheet name="Breaks y secuencias" sheetId="2" r:id="rId2"/>
+    <sheet name="Diferencia entre partidos" sheetId="3" r:id="rId3"/>
+    <sheet name="Partidos acumulados" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="28">
   <si>
     <t>BRA</t>
   </si>
@@ -87,6 +89,18 @@
   </si>
   <si>
     <t>@ECU</t>
+  </si>
+  <si>
+    <t>Minima diferencia</t>
+  </si>
+  <si>
+    <t>40 veces</t>
+  </si>
+  <si>
+    <t>Maxima diferencia</t>
+  </si>
+  <si>
+    <t>5 veces</t>
   </si>
 </sst>
 </file>
@@ -497,58 +511,58 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
         <v>8</v>
       </c>
       <c r="N2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" t="s">
-        <v>9</v>
-      </c>
       <c r="S2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -556,58 +570,58 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>5</v>
-      </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="O3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="s">
         <v>20</v>
       </c>
       <c r="R3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="S3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -615,58 +629,58 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" t="s">
-        <v>7</v>
-      </c>
       <c r="S4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -674,58 +688,58 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="P5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
         <v>19</v>
       </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" t="s">
-        <v>8</v>
-      </c>
-      <c r="P5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>2</v>
-      </c>
       <c r="R5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="S5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -733,58 +747,58 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" t="s">
-        <v>23</v>
-      </c>
       <c r="N6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" t="s">
         <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q6" t="s">
         <v>14</v>
       </c>
       <c r="R6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="S6" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -792,58 +806,58 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
       <c r="K7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s">
         <v>23</v>
       </c>
       <c r="O7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Q7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -851,58 +865,58 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I8" t="s">
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
         <v>19</v>
       </c>
-      <c r="L8" t="s">
-        <v>9</v>
-      </c>
       <c r="M8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" t="s">
         <v>17</v>
-      </c>
-      <c r="N8" t="s">
-        <v>7</v>
-      </c>
-      <c r="O8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>22</v>
-      </c>
-      <c r="S8" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -910,58 +924,58 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="L9" t="s">
         <v>22</v>
       </c>
       <c r="M9" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O9" t="s">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
       </c>
       <c r="R9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -969,10 +983,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -981,22 +995,22 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="L10" t="s">
         <v>7</v>
@@ -1005,22 +1019,22 @@
         <v>14</v>
       </c>
       <c r="N10" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="O10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P10" t="s">
         <v>9</v>
       </c>
       <c r="Q10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="R10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="S10" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1028,22 +1042,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
         <v>8</v>
@@ -1052,22 +1066,22 @@
         <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" t="s">
         <v>17</v>
       </c>
-      <c r="L11" t="s">
-        <v>20</v>
-      </c>
       <c r="M11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N11" t="s">
         <v>5</v>
       </c>
       <c r="O11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P11" t="s">
         <v>22</v>
@@ -1076,10 +1090,10 @@
         <v>7</v>
       </c>
       <c r="R11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1117,10 +1131,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1131,10 +1145,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1145,10 +1159,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1159,10 +1173,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1173,10 +1187,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1201,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1215,10 +1229,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1229,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1247,6 +1261,707 @@
       </c>
       <c r="D11">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2">
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>7</v>
+      </c>
+      <c r="Q3">
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <v>8</v>
+      </c>
+      <c r="S3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>9</v>
+      </c>
+      <c r="S4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>8</v>
+      </c>
+      <c r="R5">
+        <v>9</v>
+      </c>
+      <c r="S5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>7</v>
+      </c>
+      <c r="P6">
+        <v>7</v>
+      </c>
+      <c r="Q6">
+        <v>8</v>
+      </c>
+      <c r="R6">
+        <v>8</v>
+      </c>
+      <c r="S6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>7</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
+      <c r="P7">
+        <v>8</v>
+      </c>
+      <c r="Q7">
+        <v>8</v>
+      </c>
+      <c r="R7">
+        <v>8</v>
+      </c>
+      <c r="S7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
+      </c>
+      <c r="S8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="S9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11">
+        <v>7</v>
+      </c>
+      <c r="P11">
+        <v>8</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
+        <v>9</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregado las restricciones para darle un fixture en excel
</commit_message>
<xml_diff>
--- a/frances.xlsx
+++ b/frances.xlsx
@@ -511,58 +511,58 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" t="s">
-        <v>19</v>
-      </c>
       <c r="S2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -570,58 +570,58 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" t="s">
         <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -629,58 +629,58 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -688,58 +688,58 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" t="s">
-        <v>21</v>
-      </c>
       <c r="S5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -747,58 +747,58 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>14</v>
-      </c>
-      <c r="R6" t="s">
-        <v>8</v>
-      </c>
       <c r="S6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -806,58 +806,58 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R7" t="s">
-        <v>0</v>
-      </c>
       <c r="S7" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -865,58 +865,58 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" t="s">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
         <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>2</v>
-      </c>
-      <c r="S8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -924,58 +924,58 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
         <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" t="s">
-        <v>5</v>
-      </c>
-      <c r="N9" t="s">
-        <v>15</v>
-      </c>
-      <c r="O9" t="s">
-        <v>4</v>
-      </c>
-      <c r="P9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R9" t="s">
-        <v>3</v>
-      </c>
-      <c r="S9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -983,58 +983,58 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" t="s">
-        <v>14</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="R10" t="s">
+        <v>9</v>
+      </c>
+      <c r="S10" t="s">
         <v>17</v>
-      </c>
-      <c r="O10" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>16</v>
-      </c>
-      <c r="R10" t="s">
-        <v>18</v>
-      </c>
-      <c r="S10" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1042,58 +1042,58 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J11" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K11" t="s">
         <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="O11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11" t="s">
-        <v>15</v>
-      </c>
       <c r="S11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1159,10 +1159,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1187,10 +1187,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1201,10 +1201,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1243,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1391,13 +1391,13 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -1415,13 +1415,13 @@
         <v>6</v>
       </c>
       <c r="N2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O2">
         <v>7</v>
       </c>
       <c r="P2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q2">
         <v>8</v>
@@ -1444,19 +1444,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -1468,19 +1468,19 @@
         <v>5</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3">
         <v>6</v>
       </c>
       <c r="N3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O3">
         <v>7</v>
       </c>
       <c r="P3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q3">
         <v>8</v>
@@ -1497,55 +1497,55 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <v>4</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M4">
         <v>6</v>
       </c>
       <c r="N4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O4">
         <v>7</v>
       </c>
       <c r="P4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q4">
         <v>8</v>
       </c>
       <c r="R4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S4">
         <v>9</v>
@@ -1568,13 +1568,13 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -1592,13 +1592,13 @@
         <v>6</v>
       </c>
       <c r="N5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O5">
         <v>7</v>
       </c>
       <c r="P5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q5">
         <v>8</v>
@@ -1615,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1639,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -1663,7 +1663,7 @@
         <v>8</v>
       </c>
       <c r="R6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S6">
         <v>9</v>
@@ -1674,13 +1674,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1692,19 +1692,19 @@
         <v>3</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7">
         <v>4</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
       <c r="L7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -1716,13 +1716,13 @@
         <v>7</v>
       </c>
       <c r="P7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q7">
         <v>8</v>
       </c>
       <c r="R7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S7">
         <v>9</v>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1763,7 +1763,7 @@
         <v>5</v>
       </c>
       <c r="L8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -1804,13 +1804,13 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -1828,13 +1828,13 @@
         <v>6</v>
       </c>
       <c r="N9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O9">
         <v>7</v>
       </c>
       <c r="P9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q9">
         <v>8</v>
@@ -1851,7 +1851,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1875,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K10">
         <v>5</v>
@@ -1899,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="R10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S10">
         <v>9</v>
@@ -1922,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -1946,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="N11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O11">
         <v>7</v>

</xml_diff>

<commit_message>
nuevo run.py, con pipeline ejecucion minimax
</commit_message>
<xml_diff>
--- a/frances.xlsx
+++ b/frances.xlsx
@@ -511,58 +511,58 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="R2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
       <c r="S2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -573,13 +573,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -588,7 +588,7 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -597,13 +597,13 @@
         <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N3" t="s">
         <v>21</v>
@@ -612,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q3" t="s">
         <v>8</v>
@@ -629,58 +629,58 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
-      </c>
       <c r="P4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q4" t="s">
         <v>21</v>
       </c>
       <c r="R4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -688,58 +688,58 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
       <c r="H5" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
         <v>15</v>
       </c>
-      <c r="L5" t="s">
-        <v>7</v>
-      </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
         <v>18</v>
-      </c>
-      <c r="O5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>5</v>
-      </c>
-      <c r="R5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -747,58 +747,58 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
         <v>22</v>
       </c>
       <c r="L6" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="O6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" t="s">
         <v>19</v>
       </c>
-      <c r="P6" t="s">
-        <v>1</v>
-      </c>
       <c r="Q6" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="S6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -806,49 +806,49 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
       <c r="M7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" t="s">
         <v>14</v>
       </c>
-      <c r="O7" t="s">
-        <v>4</v>
-      </c>
       <c r="P7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="Q7" t="s">
         <v>17</v>
@@ -857,7 +857,7 @@
         <v>15</v>
       </c>
       <c r="S7" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -865,58 +865,58 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" t="s">
-        <v>21</v>
-      </c>
       <c r="N8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O8" t="s">
         <v>15</v>
       </c>
       <c r="P8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Q8" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="R8" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="S8" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -924,58 +924,58 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
       </c>
       <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" t="s">
         <v>14</v>
-      </c>
-      <c r="K9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" t="s">
-        <v>0</v>
-      </c>
-      <c r="S9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -983,58 +983,58 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="M10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
         <v>23</v>
       </c>
-      <c r="K10" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" t="s">
-        <v>0</v>
-      </c>
       <c r="P10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q10" t="s">
         <v>15</v>
       </c>
       <c r="R10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="S10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1045,52 +1045,52 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="N11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11" t="s">
         <v>14</v>
       </c>
-      <c r="J11" t="s">
-        <v>8</v>
-      </c>
-      <c r="K11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" t="s">
-        <v>3</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="Q11" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" t="s">
         <v>16</v>
-      </c>
-      <c r="O11" t="s">
-        <v>7</v>
-      </c>
-      <c r="P11" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" t="s">
-        <v>22</v>
       </c>
       <c r="S11" t="s">
         <v>1</v>
@@ -1173,10 +1173,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1215,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1391,7 +1391,7 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -1415,7 +1415,7 @@
         <v>6</v>
       </c>
       <c r="N2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O2">
         <v>7</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1527,7 +1527,7 @@
         <v>5</v>
       </c>
       <c r="L4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M4">
         <v>6</v>
@@ -1556,13 +1556,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1580,13 +1580,13 @@
         <v>4</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M5">
         <v>6</v>
@@ -1604,7 +1604,7 @@
         <v>8</v>
       </c>
       <c r="R5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S5">
         <v>9</v>
@@ -1621,19 +1621,19 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -1645,19 +1645,19 @@
         <v>5</v>
       </c>
       <c r="L6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M6">
         <v>6</v>
       </c>
       <c r="N6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O6">
         <v>7</v>
       </c>
       <c r="P6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q6">
         <v>8</v>
@@ -1686,7 +1686,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -1710,7 +1710,7 @@
         <v>6</v>
       </c>
       <c r="N7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O7">
         <v>7</v>
@@ -1733,7 +1733,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1751,13 +1751,13 @@
         <v>3</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
       <c r="J8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K8">
         <v>5</v>
@@ -1775,13 +1775,13 @@
         <v>7</v>
       </c>
       <c r="P8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q8">
         <v>8</v>
       </c>
       <c r="R8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S8">
         <v>9</v>
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1822,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="L9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M9">
         <v>6</v>
@@ -1857,13 +1857,13 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -1881,13 +1881,13 @@
         <v>5</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M10">
         <v>6</v>
       </c>
       <c r="N10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O10">
         <v>7</v>
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1940,7 +1940,7 @@
         <v>5</v>
       </c>
       <c r="L11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M11">
         <v>6</v>

</xml_diff>